<commit_message>
fixed test story failing and enrollment by african american return wrong value
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_ENR_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_ENR_2020_2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\Data_Ingestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421D18B9-3BB5-46FB-9348-8446F2A233A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6982EA-1E42-4ABB-96F9-5527D0A23385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>nonresident-alien</t>
   </si>
   <si>
-    <t>african-american</t>
-  </si>
-  <si>
     <t>american-indian</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>two or more races</t>
+  </si>
+  <si>
+    <t>african american</t>
   </si>
 </sst>
 </file>
@@ -473,25 +473,25 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -2531,7 +2531,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2553,7 +2553,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -2562,22 +2562,22 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
         <v>12</v>

</xml_diff>